<commit_message>
Update Populationsdaten (2012 - 2021).xlsx
</commit_message>
<xml_diff>
--- a/Populationsdaten (2012 - 2021).xlsx
+++ b/Populationsdaten (2012 - 2021).xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
-    <t>Province</t>
-  </si>
-  <si>
     <t>Bangkok</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>Narathiwat</t>
+  </si>
+  <si>
+    <t>Reporting_areas</t>
   </si>
 </sst>
 </file>
@@ -655,9 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -669,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2">
         <v>2012</v>
@@ -701,7 +699,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4">
         <v>372868</v>
@@ -733,7 +731,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
         <v>283972</v>
@@ -765,7 +763,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="4">
         <v>5674202</v>
@@ -797,7 +795,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4">
         <v>410124</v>
@@ -829,7 +827,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4">
         <v>1562912</v>
@@ -861,7 +859,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4">
         <v>682545</v>
@@ -893,7 +891,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4">
         <v>333214</v>
@@ -925,7 +923,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4">
         <v>1130228</v>
@@ -957,7 +955,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4">
         <v>519333</v>
@@ -989,7 +987,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>1650893</v>
@@ -1021,7 +1019,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4">
         <v>1199539</v>
@@ -1053,7 +1051,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
         <v>1351329</v>
@@ -1085,7 +1083,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4">
         <v>493746</v>
@@ -1117,7 +1115,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="4">
         <v>983370</v>
@@ -1149,7 +1147,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4">
         <v>726782</v>
@@ -1181,7 +1179,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="4">
         <v>838591</v>
@@ -1213,7 +1211,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="4">
         <v>1770441</v>
@@ -1245,7 +1243,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="4">
         <v>441503</v>
@@ -1277,7 +1275,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>757173</v>
@@ -1309,7 +1307,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4">
         <v>404313</v>
@@ -1341,7 +1339,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="4">
         <v>627354</v>
@@ -1373,7 +1371,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="4">
         <v>757093</v>
@@ -1405,7 +1403,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="4">
         <v>244202</v>
@@ -1437,7 +1435,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4">
         <v>942442</v>
@@ -1469,7 +1467,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="4">
         <v>341725</v>
@@ -1501,7 +1499,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="4">
         <v>254502</v>
@@ -1533,7 +1531,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="4">
         <v>870340</v>
@@ -1565,7 +1563,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="4">
         <v>706559</v>
@@ -1597,7 +1595,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="4">
         <v>2593246</v>
@@ -1629,7 +1627,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="4">
         <v>1072516</v>
@@ -1661,7 +1659,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4">
         <v>1530479</v>
@@ -1693,7 +1691,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="4">
         <v>477142</v>
@@ -1725,7 +1723,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="4">
         <v>752384</v>
@@ -1757,7 +1755,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="4">
         <v>503811</v>
@@ -1789,7 +1787,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="4">
         <v>511155</v>
@@ -1821,7 +1819,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" s="4">
         <v>1132150</v>
@@ -1853,7 +1851,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="4">
         <v>1022367</v>
@@ -1885,7 +1883,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="4">
         <v>667550</v>
@@ -1917,7 +1915,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4">
         <v>256212</v>
@@ -1949,7 +1947,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="4">
         <v>512777</v>
@@ -1981,7 +1979,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="4">
         <v>487296</v>
@@ -2013,7 +2011,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" s="4">
         <v>467476</v>
@@ -2045,7 +2043,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4">
         <v>992255</v>
@@ -2077,7 +2075,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="4">
         <v>549541</v>
@@ -2109,7 +2107,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="4">
         <v>852864</v>
@@ -2141,7 +2139,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="4">
         <v>790581</v>
@@ -2173,7 +2171,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="4">
         <v>458178</v>
@@ -2205,7 +2203,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="4">
         <v>357376</v>
@@ -2237,7 +2235,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" s="4">
         <v>471711</v>
@@ -2269,7 +2267,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B51" s="4">
         <v>514809</v>
@@ -2301,7 +2299,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" s="4">
         <v>183248</v>
@@ -2333,7 +2331,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="4">
         <v>844658</v>
@@ -2365,7 +2363,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="4">
         <v>643506</v>
@@ -2397,7 +2395,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="4">
         <v>1306814</v>
@@ -2429,7 +2427,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B56" s="4">
         <v>546969</v>
@@ -2461,7 +2459,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="4">
         <v>1126263</v>
@@ -2493,7 +2491,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" s="4">
         <v>1213262</v>
@@ -2525,7 +2523,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59" s="4">
         <v>503956</v>
@@ -2557,7 +2555,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" s="4">
         <v>194064</v>
@@ -2589,7 +2587,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61" s="4">
         <v>623071</v>
@@ -2621,7 +2619,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" s="4">
         <v>303674</v>
@@ -2653,7 +2651,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B63" s="4">
         <v>1455287</v>
@@ -2685,7 +2683,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B64" s="4">
         <v>213402</v>
@@ -2717,7 +2715,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="4">
         <v>1372792</v>
@@ -2749,7 +2747,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="4">
         <v>602053</v>
@@ -2781,7 +2779,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="4">
         <v>846181</v>
@@ -2813,7 +2811,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="4">
         <v>1017676</v>
@@ -2845,7 +2843,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" s="4">
         <v>1383338</v>
@@ -2877,7 +2875,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B70" s="4">
         <v>528531</v>
@@ -2909,7 +2907,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="4">
         <v>629314</v>
@@ -2941,7 +2939,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72" s="4">
         <v>222434</v>
@@ -2973,7 +2971,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B73" s="4">
         <v>1821489</v>
@@ -3005,7 +3003,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B74" s="4">
         <v>1552703</v>
@@ -3037,7 +3035,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B75" s="4">
         <v>328492</v>
@@ -3069,7 +3067,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="4">
         <v>461167</v>
@@ -3101,7 +3099,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="4">
         <v>497290</v>
@@ -3133,7 +3131,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B78" s="6">
         <v>539560</v>

</xml_diff>